<commit_message>
update institute example file and doc
</commit_message>
<xml_diff>
--- a/src/assets/upload_examples/institutes.xlsx
+++ b/src/assets/upload_examples/institutes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">INSTCODE</t>
   </si>
@@ -31,6 +31,30 @@
     <t xml:space="preserve">TYPE</t>
   </si>
   <si>
+    <t xml:space="preserve">STREET_POB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CITY_STATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIP_CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLLECTIONS</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP004</t>
   </si>
   <si>
@@ -40,6 +64,24 @@
     <t xml:space="preserve">Governmental</t>
   </si>
   <si>
+    <t xml:space="preserve">my address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">curator@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The curator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pepper, tomato</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESP026</t>
   </si>
   <si>
@@ -50,12 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">La mayora Genebank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PeruExpedition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expedicion a peru</t>
   </si>
 </sst>
 </file>
@@ -65,11 +101,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +122,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,8 +173,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,22 +195,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -175,49 +224,93 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>988338822</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="curator@example.com"/>
+    <hyperlink ref="I2" r:id="rId2" display="https://example.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>